<commit_message>
updated data for missing character traits and added manuscript
</commit_message>
<xml_diff>
--- a/trait_data/Lizard_Trait_Data.xlsx
+++ b/trait_data/Lizard_Trait_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/980b074849a8c2a3/Documents/lizard_brain_evolution/trait_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="123" documentId="13_ncr:40009_{7589B547-1B80-4F32-BD99-4048CA94C5B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67CACBA9-40C9-4444-852A-2AB623181B3F}"/>
+  <xr:revisionPtr revIDLastSave="148" documentId="13_ncr:40009_{7589B547-1B80-4F32-BD99-4048CA94C5B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF09BA3E-3EF1-484A-B6AD-A22C5FC46004}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16354" yWindow="-3711" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lizard_Trait_Data_2021-10-08" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="110">
   <si>
     <t>Id</t>
   </si>
@@ -52,9 +52,6 @@
     <t>substrate</t>
   </si>
   <si>
-    <t>diet</t>
-  </si>
-  <si>
     <t>foraging_mode</t>
   </si>
   <si>
@@ -88,9 +85,6 @@
     <t>Terrestrial</t>
   </si>
   <si>
-    <t>Carnivorous</t>
-  </si>
-  <si>
     <t>active_foraging</t>
   </si>
   <si>
@@ -128,9 +122,6 @@
   </si>
   <si>
     <t>Arboreal_Saxicolous</t>
-  </si>
-  <si>
-    <t>Omnivorous</t>
   </si>
   <si>
     <t>sit_and_wait</t>
@@ -387,64 +378,25 @@
     <t>Bowker 1984; Mesquita et al. 2016</t>
   </si>
   <si>
-    <t>unsuccesful in finding data</t>
-  </si>
-  <si>
     <t>gardinitiative.org</t>
   </si>
   <si>
-    <t>hatchling_mass</t>
-  </si>
-  <si>
     <t>reference</t>
   </si>
   <si>
-    <t>mean_Tb</t>
-  </si>
-  <si>
-    <t>gardinitiative.org; Withers 1981</t>
-  </si>
-  <si>
-    <t>gardinitiative.org; Muchlinski et al. 1995; Bowker 1984</t>
-  </si>
-  <si>
-    <t>gardinitiative.org; Galan and Salvador 2006; Brown and Roberts 2008; Hailey and Elliot 1995</t>
-  </si>
-  <si>
-    <t>gardinitiative.org; Savage 2002; Hirth 1963; Hirth 1965</t>
-  </si>
-  <si>
-    <t>gardinitiative.org; Hailey and Elliot 1995; Lopez 2009</t>
-  </si>
-  <si>
-    <t>gardinitiative.org; Andrews 2008; Avery 1982; Dimaki et al. 2000</t>
-  </si>
-  <si>
-    <t>gardinitiative.org; Meiri, own data</t>
-  </si>
-  <si>
-    <t>gardinitiatve.org; Avery 1982; Alcala 1966</t>
-  </si>
-  <si>
-    <t>gardinitiative.org; MacMillen et al. 1989, Melville and Schulte 2001, Greer 1989</t>
-  </si>
-  <si>
-    <t>gardinitiative.org; Meek 1986, Meiri, own data</t>
-  </si>
-  <si>
-    <t>gardinitiative.org; Verwaijen and Van Damme 2007</t>
-  </si>
-  <si>
-    <t>gardinitiative.org; Andrews 2008</t>
-  </si>
-  <si>
-    <t>gardinitiative.org; Rocha et al. 2009, Kiefer et al. 2005</t>
-  </si>
-  <si>
     <t>updated 10/14/2021</t>
   </si>
   <si>
     <t xml:space="preserve">Montechiaro 2011 North Western Journal of Zoology </t>
+  </si>
+  <si>
+    <t>Macri et al. 2019 Nat Comm</t>
+  </si>
+  <si>
+    <t>inferred/imputed</t>
+  </si>
+  <si>
+    <t>Unknown</t>
   </si>
 </sst>
 </file>
@@ -1044,7 +996,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1098,6 +1050,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1455,11 +1410,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM30"/>
+  <dimension ref="A1:AG30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A5" sqref="A5"/>
+      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1480,33 +1435,27 @@
     <col min="14" max="14" width="11.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.6640625" style="4" customWidth="1"/>
     <col min="16" max="16" width="19" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19" style="4" customWidth="1"/>
+    <col min="17" max="17" width="24.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.88671875" style="8" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="32.77734375" style="4" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="28" style="8" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="33.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.88671875" style="4" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="33.33203125" style="4" customWidth="1"/>
-    <col min="24" max="24" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="45.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="44.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18" style="8" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18" style="4" customWidth="1"/>
-    <col min="30" max="30" width="10.21875" style="8" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.21875" style="4" customWidth="1"/>
-    <col min="32" max="32" width="14.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.44140625" style="4" customWidth="1"/>
-    <col min="35" max="35" width="63.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="22.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="22.5546875" style="4" customWidth="1"/>
-    <col min="38" max="38" width="21.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="18.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="40" max="16384" width="8.88671875" style="8"/>
+    <col min="24" max="24" width="13.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="44.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18" style="8" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18" style="4" customWidth="1"/>
+    <col min="28" max="28" width="10.21875" style="8" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.21875" style="4" customWidth="1"/>
+    <col min="30" max="30" width="22.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="22.5546875" style="4" customWidth="1"/>
+    <col min="32" max="32" width="21.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="18.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="34" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1514,13 +1463,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -1530,7 +1479,7 @@
         <v>3</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
@@ -1547,89 +1496,75 @@
       <c r="P1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="2"/>
+      <c r="Q1" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="R1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="U1" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="W1" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="X1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="X1" s="17" t="s">
         <v>10</v>
       </c>
       <c r="Y1" s="2"/>
-      <c r="Z1" s="17" t="s">
+      <c r="Z1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="2"/>
+      <c r="AA1" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="AB1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AC1" s="2" t="s">
-        <v>94</v>
-      </c>
+      <c r="AC1" s="2"/>
       <c r="AD1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AE1" s="2"/>
-      <c r="AF1" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="AG1" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="AH1" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="AI1" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AE1" s="17"/>
+      <c r="AF1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AK1" s="17"/>
-      <c r="AL1" s="1" t="s">
+      <c r="AG1" s="18"/>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="AM1" s="18"/>
-    </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="B2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="C2" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D2" s="5">
         <v>41.11</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F2" s="5">
         <v>25.77</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J2" s="5">
         <v>58</v>
@@ -1644,85 +1579,79 @@
       </c>
       <c r="O2" s="6"/>
       <c r="P2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="R2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="T2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="T2" s="13" t="s">
+      <c r="U2" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="V2" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="X2" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="U2" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="V2" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="W2" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="X2" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="Y2" s="6"/>
       <c r="Z2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="5">
+        <v>2.8</v>
+      </c>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="5" t="s">
+      <c r="AE2" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="AF2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="5">
-        <v>2.8</v>
-      </c>
-      <c r="AE2" s="6"/>
-      <c r="AF2" s="15"/>
-      <c r="AG2" s="6"/>
-      <c r="AH2" s="15"/>
-      <c r="AI2" s="15"/>
-      <c r="AJ2" s="5" t="s">
+      <c r="AG2" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="AK2" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="AL2" s="5" t="s">
+      <c r="B3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AM2" s="7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="C3" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D3" s="5">
         <v>33.24</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F3" s="5">
         <v>21.77</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J3" s="5">
         <v>295</v>
@@ -1737,91 +1666,77 @@
       </c>
       <c r="O3" s="6"/>
       <c r="P3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="T3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="U3" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="V3" s="15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Y3" s="6"/>
       <c r="Z3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA3" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB3" s="5">
+        <v>3</v>
+      </c>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC3" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AD3" s="5">
-        <v>3</v>
-      </c>
       <c r="AE3" s="6"/>
-      <c r="AF3" s="15">
-        <v>0.16</v>
-      </c>
-      <c r="AG3" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH3" s="15">
-        <v>21.8</v>
-      </c>
-      <c r="AI3" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="AJ3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK3" s="6"/>
-      <c r="AL3" s="5" t="s">
+      <c r="AF3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG3" s="7"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AM3" s="7"/>
-    </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="C4" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D4" s="5">
         <v>4.2</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F4" s="5">
         <v>15.61</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J4" s="5">
         <v>150</v>
@@ -1836,74 +1751,60 @@
       </c>
       <c r="O4" s="6"/>
       <c r="P4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="V4" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="W4" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="X4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="S4" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="T4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="U4" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="V4" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="W4" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="X4" s="5" t="s">
+      <c r="Y4" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA4" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB4" s="5">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG4" s="7"/>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="Y4" s="6"/>
-      <c r="Z4" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="AA4" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="AB4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC4" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AD4" s="5">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="AE4" s="6"/>
-      <c r="AF4" s="15">
-        <v>-0.19</v>
-      </c>
-      <c r="AG4" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH4" s="15">
-        <v>35.9</v>
-      </c>
-      <c r="AI4" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="AJ4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK4" s="6"/>
-      <c r="AL4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="AM4" s="7"/>
-    </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="5">
@@ -1915,87 +1816,87 @@
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="5">
         <v>500</v>
       </c>
       <c r="K5" s="6"/>
-      <c r="L5" s="5" t="s">
-        <v>41</v>
+      <c r="L5" s="19" t="s">
+        <v>38</v>
       </c>
       <c r="M5" s="6"/>
-      <c r="N5" s="5" t="s">
-        <v>41</v>
+      <c r="N5" s="19" t="s">
+        <v>38</v>
       </c>
       <c r="O5" s="6"/>
       <c r="P5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="U5" s="6"/>
+      <c r="V5" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="U5" s="6"/>
-      <c r="V5" s="15"/>
       <c r="W5" s="6"/>
       <c r="X5" s="5" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="Y5" s="6"/>
       <c r="Z5" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AA5" s="6"/>
-      <c r="AB5" s="5" t="s">
-        <v>24</v>
+      <c r="AB5" s="19" t="s">
+        <v>38</v>
       </c>
       <c r="AC5" s="6"/>
       <c r="AD5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE5" s="6"/>
+      <c r="AF5" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AE5" s="6"/>
-      <c r="AF5" s="15"/>
-      <c r="AG5" s="6"/>
-      <c r="AH5" s="15"/>
-      <c r="AI5" s="15"/>
-      <c r="AJ5" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="AK5" s="6"/>
-      <c r="AL5" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM5" s="7"/>
+      <c r="AG5" s="7"/>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D6" s="5">
         <v>50.12</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F6" s="5">
         <v>8.1</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J6" s="5">
         <v>291</v>
@@ -2010,93 +1911,79 @@
       </c>
       <c r="O6" s="6"/>
       <c r="P6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="R6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="5" t="s">
+      <c r="S6" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="T6" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="U6" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="V6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="S6" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="T6" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="U6" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="V6" s="15" t="s">
+      <c r="W6" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="X6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="W6" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="X6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y6" s="6"/>
+      <c r="Y6" s="6" t="s">
+        <v>92</v>
+      </c>
       <c r="Z6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA6" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB6" s="5">
+        <v>9.48</v>
+      </c>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="AA6" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="AB6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC6" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AD6" s="5">
-        <v>9.48</v>
-      </c>
       <c r="AE6" s="6"/>
-      <c r="AF6" s="15">
-        <v>-0.4</v>
-      </c>
-      <c r="AG6" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH6" s="15">
-        <v>24.3</v>
-      </c>
-      <c r="AI6" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="AJ6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK6" s="6"/>
-      <c r="AL6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="AM6" s="7"/>
+      <c r="AF6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG6" s="7"/>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D7" s="5">
         <v>0.37</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F7" s="5">
         <v>-60.46</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J7" s="5">
         <v>80</v>
@@ -2111,81 +1998,75 @@
       </c>
       <c r="O7" s="6"/>
       <c r="P7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="R7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="S7" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T7" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="U7" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="V7" s="15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="W7" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="X7" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Y7" s="6"/>
       <c r="Z7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="AA7" s="6"/>
-      <c r="AB7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC7" s="6"/>
-      <c r="AD7" s="5">
-        <v>1</v>
-      </c>
       <c r="AE7" s="6"/>
-      <c r="AF7" s="15"/>
-      <c r="AG7" s="6"/>
-      <c r="AH7" s="15"/>
-      <c r="AI7" s="15"/>
-      <c r="AJ7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK7" s="6"/>
-      <c r="AL7" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM7" s="7"/>
+      <c r="AF7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG7" s="7"/>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D8" s="5">
         <v>16.82</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F8" s="5">
         <v>-91.18</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J8" s="5">
         <v>225</v>
@@ -2200,93 +2081,79 @@
       </c>
       <c r="O8" s="6"/>
       <c r="P8" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q8" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="R8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S8" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="T8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="U8" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="V8" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="T8" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="U8" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="V8" s="15" t="s">
-        <v>93</v>
-      </c>
       <c r="W8" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="X8" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y8" s="6"/>
+        <v>34</v>
+      </c>
+      <c r="Y8" s="6" t="s">
+        <v>101</v>
+      </c>
       <c r="Z8" s="5" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="AA8" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="AB8" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB8" s="5">
+        <v>5.4</v>
+      </c>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AC8" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AD8" s="5">
-        <v>5.4</v>
-      </c>
-      <c r="AE8" s="6"/>
-      <c r="AF8" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="AG8" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH8" s="15">
-        <v>36.200000000000003</v>
-      </c>
-      <c r="AI8" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="AJ8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK8" s="6"/>
-      <c r="AL8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="AM8" s="7"/>
+      <c r="AG8" s="7"/>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D9" s="5">
         <v>37.92</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F9" s="5">
         <v>-4.57</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J9" s="5">
         <v>254</v>
@@ -2301,91 +2168,77 @@
       </c>
       <c r="O9" s="6"/>
       <c r="P9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="S9" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="T9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="S9" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="T9" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="U9" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="V9" s="15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="W9" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="X9" s="5" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="Y9" s="6"/>
       <c r="Z9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA9" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB9" s="5">
+        <v>2</v>
+      </c>
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="AA9" s="6"/>
-      <c r="AB9" s="5" t="s">
+      <c r="AE9" s="6"/>
+      <c r="AF9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AC9" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AD9" s="5">
-        <v>2</v>
-      </c>
-      <c r="AE9" s="6"/>
-      <c r="AF9" s="15">
-        <v>-0.39</v>
-      </c>
-      <c r="AG9" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH9" s="15">
-        <v>22.8</v>
-      </c>
-      <c r="AI9" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="AJ9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK9" s="6"/>
-      <c r="AL9" s="5" t="s">
+      <c r="AG9" s="7"/>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AM9" s="7"/>
-    </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="C10" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D10" s="5">
         <v>33.32</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F10" s="5">
         <v>17.739999999999998</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J10" s="5">
         <v>103.6</v>
@@ -2400,93 +2253,79 @@
       </c>
       <c r="O10" s="6"/>
       <c r="P10" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q10" s="6"/>
+        <v>51</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="R10" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S10" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="T10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="U10" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="V10" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="T10" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="U10" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="V10" s="15" t="s">
-        <v>93</v>
-      </c>
       <c r="W10" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="X10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y10" s="6"/>
+        <v>53</v>
+      </c>
+      <c r="Y10" s="6" t="s">
+        <v>100</v>
+      </c>
       <c r="Z10" s="5" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="AA10" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="AB10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC10" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AD10" s="5">
+      <c r="AB10" s="5">
         <v>12.5</v>
       </c>
+      <c r="AC10" s="6"/>
+      <c r="AD10" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="AE10" s="6"/>
-      <c r="AF10" s="15">
-        <v>-0.45</v>
-      </c>
-      <c r="AG10" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH10" s="15">
-        <v>27.2</v>
-      </c>
-      <c r="AI10" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="AJ10" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="AK10" s="6"/>
-      <c r="AL10" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="AM10" s="7"/>
+      <c r="AF10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG10" s="7"/>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D11" s="5">
         <v>40.6</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F11" s="5">
         <v>12.65</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J11" s="5">
         <v>210</v>
@@ -2501,81 +2340,75 @@
       </c>
       <c r="O11" s="6"/>
       <c r="P11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q11" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="R11" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="S11" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T11" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="U11" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="V11" s="15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="W11" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="X11" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Y11" s="6"/>
       <c r="Z11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA11" s="6"/>
+      <c r="AB11" s="5">
+        <v>7.4</v>
+      </c>
+      <c r="AC11" s="6"/>
+      <c r="AD11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="AA11" s="6"/>
-      <c r="AB11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC11" s="6"/>
-      <c r="AD11" s="5">
-        <v>7.4</v>
-      </c>
       <c r="AE11" s="6"/>
-      <c r="AF11" s="15"/>
-      <c r="AG11" s="6"/>
-      <c r="AH11" s="15"/>
-      <c r="AI11" s="15"/>
-      <c r="AJ11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK11" s="6"/>
-      <c r="AL11" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="AM11" s="7"/>
+      <c r="AF11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG11" s="7"/>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D12" s="5">
         <v>28.89</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F12" s="5">
         <v>25.62</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J12" s="5">
         <v>116</v>
@@ -2590,91 +2423,77 @@
       </c>
       <c r="O12" s="6"/>
       <c r="P12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q12" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="R12" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="S12" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T12" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="U12" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="V12" s="15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="W12" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="X12" s="5" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="Y12" s="6"/>
       <c r="Z12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA12" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB12" s="5">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="AC12" s="6"/>
+      <c r="AD12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="AA12" s="6"/>
-      <c r="AB12" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC12" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AD12" s="5">
-        <v>4.3499999999999996</v>
-      </c>
       <c r="AE12" s="6"/>
-      <c r="AF12" s="15">
-        <v>-0.27</v>
-      </c>
-      <c r="AG12" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH12" s="15">
-        <v>26.6</v>
-      </c>
-      <c r="AI12" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ12" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK12" s="6"/>
-      <c r="AL12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="AM12" s="7"/>
+      <c r="AF12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG12" s="7"/>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D13" s="5">
         <v>2.92</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F13" s="5">
         <v>107.45</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J13" s="5">
         <v>150</v>
@@ -2689,83 +2508,77 @@
       </c>
       <c r="O13" s="6"/>
       <c r="P13" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q13" s="6"/>
+        <v>51</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="R13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S13" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="T13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="U13" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="V13" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="T13" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="U13" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="V13" s="15" t="s">
-        <v>93</v>
-      </c>
       <c r="W13" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="X13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y13" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="Y13" s="6"/>
-      <c r="Z13" s="5" t="s">
+      <c r="AA13" s="6"/>
+      <c r="AB13" s="5">
+        <v>6.17</v>
+      </c>
+      <c r="AC13" s="6"/>
+      <c r="AD13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="AA13" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="AB13" s="5" t="s">
+      <c r="AE13" s="6"/>
+      <c r="AF13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AC13" s="6"/>
-      <c r="AD13" s="5">
-        <v>6.17</v>
-      </c>
-      <c r="AE13" s="6"/>
-      <c r="AF13" s="15"/>
-      <c r="AG13" s="6"/>
-      <c r="AH13" s="15"/>
-      <c r="AI13" s="15"/>
-      <c r="AJ13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK13" s="6"/>
-      <c r="AL13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="AM13" s="7"/>
+      <c r="AG13" s="7"/>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D14" s="5">
         <v>7.35</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F14" s="5">
         <v>110.24</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J14" s="5">
         <v>96</v>
@@ -2780,91 +2593,77 @@
       </c>
       <c r="O14" s="6"/>
       <c r="P14" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q14" s="6"/>
+        <v>62</v>
+      </c>
+      <c r="Q14" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="R14" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S14" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="T14" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="U14" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="V14" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="T14" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="U14" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="V14" s="15" t="s">
-        <v>93</v>
-      </c>
       <c r="W14" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="X14" s="5" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="Y14" s="6"/>
       <c r="Z14" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA14" s="6"/>
-      <c r="AB14" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC14" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AD14" s="5">
+        <v>22</v>
+      </c>
+      <c r="AA14" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB14" s="5">
         <v>4.5</v>
       </c>
+      <c r="AC14" s="6"/>
+      <c r="AD14" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="AE14" s="6"/>
-      <c r="AF14" s="15">
-        <v>-0.4</v>
-      </c>
-      <c r="AG14" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH14" s="15">
-        <v>29.3</v>
-      </c>
-      <c r="AI14" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="AJ14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK14" s="6"/>
-      <c r="AL14" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM14" s="7"/>
+      <c r="AF14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG14" s="7"/>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D15" s="5">
         <v>28.68</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F15" s="5">
         <v>70.510000000000005</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J15" s="5">
         <v>170</v>
@@ -2879,83 +2678,77 @@
       </c>
       <c r="O15" s="6"/>
       <c r="P15" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q15" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="Q15" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="R15" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="S15" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="U15" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="V15" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="W15" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="X15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="U15" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="V15" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="W15" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="X15" s="5" t="s">
+      <c r="Y15" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z15" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="Y15" s="6"/>
-      <c r="Z15" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA15" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="AB15" s="5" t="s">
-        <v>24</v>
+      <c r="AA15" s="6"/>
+      <c r="AB15" s="5">
+        <v>2.38</v>
       </c>
       <c r="AC15" s="6"/>
-      <c r="AD15" s="5">
-        <v>2.38</v>
+      <c r="AD15" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="AE15" s="6"/>
-      <c r="AF15" s="15"/>
-      <c r="AG15" s="6"/>
-      <c r="AH15" s="15"/>
-      <c r="AI15" s="15"/>
-      <c r="AJ15" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="AK15" s="6"/>
-      <c r="AL15" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="AM15" s="7"/>
+      <c r="AF15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG15" s="7"/>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D16" s="5">
         <v>13.93</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F16" s="5">
         <v>104.18</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J16" s="5">
         <v>220</v>
@@ -2970,83 +2763,77 @@
       </c>
       <c r="O16" s="6"/>
       <c r="P16" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q16" s="6"/>
+        <v>51</v>
+      </c>
+      <c r="Q16" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="R16" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="S16" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="T16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U16" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="V16" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="W16" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="X16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y16" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA16" s="6"/>
+      <c r="AB16" s="5">
+        <v>2</v>
+      </c>
+      <c r="AC16" s="6"/>
+      <c r="AD16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE16" s="6"/>
+      <c r="AF16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG16" s="7"/>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="S16" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="T16" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="U16" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="V16" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="W16" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="X16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y16" s="6"/>
-      <c r="Z16" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA16" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="AB16" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC16" s="6"/>
-      <c r="AD16" s="5">
-        <v>2</v>
-      </c>
-      <c r="AE16" s="6"/>
-      <c r="AF16" s="15"/>
-      <c r="AG16" s="6"/>
-      <c r="AH16" s="15"/>
-      <c r="AI16" s="15"/>
-      <c r="AJ16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK16" s="6"/>
-      <c r="AL16" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM16" s="7"/>
-    </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>70</v>
-      </c>
       <c r="C17" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D17" s="5">
         <v>32.450000000000003</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F17" s="5">
         <v>115.76</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J17" s="5">
         <v>75</v>
@@ -3061,81 +2848,75 @@
       </c>
       <c r="O17" s="6"/>
       <c r="P17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q17" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="Q17" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="R17" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="S17" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T17" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="U17" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="V17" s="15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="W17" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="X17" s="5" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="Y17" s="6"/>
       <c r="Z17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA17" s="6"/>
+      <c r="AB17" s="5">
+        <v>4</v>
+      </c>
+      <c r="AC17" s="6"/>
+      <c r="AD17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="AA17" s="6"/>
-      <c r="AB17" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC17" s="6"/>
-      <c r="AD17" s="5">
-        <v>4</v>
-      </c>
       <c r="AE17" s="6"/>
-      <c r="AF17" s="15"/>
-      <c r="AG17" s="6"/>
-      <c r="AH17" s="15"/>
-      <c r="AI17" s="15"/>
-      <c r="AJ17" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK17" s="6"/>
-      <c r="AL17" s="5" t="s">
+      <c r="AF17" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG17" s="7"/>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AM17" s="7"/>
-    </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="C18" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D18" s="5">
         <v>4.31316948015</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F18" s="5">
         <v>8.58</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J18" s="5">
         <v>180</v>
@@ -3150,81 +2931,75 @@
       </c>
       <c r="O18" s="6"/>
       <c r="P18" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q18" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="Q18" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="R18" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="S18" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T18" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U18" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="V18" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="W18" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="X18" s="5" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="Y18" s="6"/>
       <c r="Z18" s="5" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
       <c r="AA18" s="6"/>
-      <c r="AB18" s="5" t="s">
-        <v>24</v>
+      <c r="AB18" s="5">
+        <v>10</v>
       </c>
       <c r="AC18" s="6"/>
-      <c r="AD18" s="5">
-        <v>10</v>
+      <c r="AD18" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="AE18" s="6"/>
-      <c r="AF18" s="15"/>
-      <c r="AG18" s="6"/>
-      <c r="AH18" s="15"/>
-      <c r="AI18" s="15"/>
-      <c r="AJ18" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK18" s="6"/>
-      <c r="AL18" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM18" s="7"/>
+      <c r="AF18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG18" s="7"/>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D19" s="5">
         <v>2.4500000000000002</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F19" s="5">
         <v>34.36</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J19" s="5">
         <v>43</v>
@@ -3239,83 +3014,77 @@
       </c>
       <c r="O19" s="6"/>
       <c r="P19" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q19" s="6"/>
+        <v>51</v>
+      </c>
+      <c r="Q19" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="R19" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S19" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="T19" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="U19" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="V19" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="T19" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="U19" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="V19" s="15" t="s">
-        <v>93</v>
-      </c>
       <c r="W19" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="X19" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y19" s="6"/>
+        <v>53</v>
+      </c>
+      <c r="Y19" s="6" t="s">
+        <v>97</v>
+      </c>
       <c r="Z19" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA19" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="AB19" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="AA19" s="6"/>
+      <c r="AB19" s="5">
+        <v>2</v>
       </c>
       <c r="AC19" s="6"/>
-      <c r="AD19" s="5">
-        <v>2</v>
+      <c r="AD19" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="AE19" s="6"/>
-      <c r="AF19" s="15"/>
-      <c r="AG19" s="6"/>
-      <c r="AH19" s="15"/>
-      <c r="AI19" s="15"/>
-      <c r="AJ19" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK19" s="6"/>
-      <c r="AL19" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM19" s="7"/>
+      <c r="AF19" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG19" s="7"/>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D20" s="5">
         <v>8.6</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F20" s="5">
         <v>36.409999999999997</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J20" s="5">
         <v>145</v>
@@ -3330,83 +3099,77 @@
       </c>
       <c r="O20" s="6"/>
       <c r="P20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q20" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="R20" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="S20" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="T20" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="5" t="s">
+      <c r="U20" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="V20" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="W20" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="X20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y20" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA20" s="6"/>
+      <c r="AB20" s="5">
+        <v>4.25</v>
+      </c>
+      <c r="AC20" s="6"/>
+      <c r="AD20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE20" s="6"/>
+      <c r="AF20" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="S20" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="T20" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="U20" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="V20" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="W20" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="X20" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y20" s="6"/>
-      <c r="Z20" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA20" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="AB20" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC20" s="6"/>
-      <c r="AD20" s="5">
-        <v>4.25</v>
-      </c>
-      <c r="AE20" s="6"/>
-      <c r="AF20" s="15"/>
-      <c r="AG20" s="6"/>
-      <c r="AH20" s="15"/>
-      <c r="AI20" s="15"/>
-      <c r="AJ20" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK20" s="6"/>
-      <c r="AL20" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM20" s="7"/>
+      <c r="AG20" s="7"/>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D21" s="5">
         <v>23.53</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F21" s="5">
         <v>-50.52</v>
       </c>
       <c r="G21" s="6"/>
       <c r="H21" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J21" s="5">
         <v>300</v>
@@ -3421,83 +3184,75 @@
       </c>
       <c r="O21" s="6"/>
       <c r="P21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q21" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="R21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="5" t="s">
+      <c r="S21" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="T21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="S21" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="T21" s="5" t="s">
+      <c r="U21" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="V21" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="W21" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="X21" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="U21" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="V21" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="W21" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="X21" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y21" s="6" t="s">
-        <v>125</v>
-      </c>
+      <c r="Y21" s="6"/>
       <c r="Z21" s="5" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="AA21" s="6"/>
-      <c r="AB21" s="5" t="s">
-        <v>32</v>
+      <c r="AB21" s="5">
+        <v>5.55</v>
       </c>
       <c r="AC21" s="6"/>
-      <c r="AD21" s="5">
-        <v>5.55</v>
+      <c r="AD21" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="AE21" s="6"/>
-      <c r="AF21" s="15"/>
-      <c r="AG21" s="6"/>
-      <c r="AH21" s="15"/>
-      <c r="AI21" s="15"/>
-      <c r="AJ21" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="AK21" s="6"/>
-      <c r="AL21" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="AM21" s="7"/>
+      <c r="AF21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG21" s="7"/>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D22" s="5">
         <v>14.02</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F22" s="5">
         <v>49.37</v>
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J22" s="5">
         <v>118</v>
@@ -3512,62 +3267,56 @@
       </c>
       <c r="O22" s="6"/>
       <c r="P22" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q22" s="6"/>
+        <v>51</v>
+      </c>
+      <c r="Q22" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="R22" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S22" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="T22" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="U22" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="V22" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="T22" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="U22" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="V22" s="15" t="s">
-        <v>93</v>
-      </c>
       <c r="W22" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="X22" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Y22" s="6"/>
       <c r="Z22" s="5" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="AA22" s="6"/>
-      <c r="AB22" s="5" t="s">
-        <v>24</v>
+      <c r="AB22" s="5">
+        <v>2</v>
       </c>
       <c r="AC22" s="6"/>
-      <c r="AD22" s="5">
-        <v>2</v>
+      <c r="AD22" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="AE22" s="6"/>
-      <c r="AF22" s="15"/>
-      <c r="AG22" s="6"/>
-      <c r="AH22" s="15"/>
-      <c r="AI22" s="15"/>
-      <c r="AJ22" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK22" s="6"/>
-      <c r="AL22" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM22" s="7"/>
+      <c r="AF22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG22" s="7"/>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="5">
@@ -3579,7 +3328,7 @@
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I23" s="6"/>
       <c r="J23" s="5">
@@ -3590,76 +3339,76 @@
         <v>72.3</v>
       </c>
       <c r="M23" s="6"/>
-      <c r="N23" s="5" t="s">
-        <v>41</v>
+      <c r="N23" s="19" t="s">
+        <v>38</v>
       </c>
       <c r="O23" s="6"/>
       <c r="P23" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="Q23" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="R23" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="S23" s="6" t="s">
+        <v>108</v>
+      </c>
       <c r="T23" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U23" s="6"/>
-      <c r="V23" s="15"/>
+      <c r="V23" s="15" t="s">
+        <v>20</v>
+      </c>
       <c r="W23" s="6"/>
       <c r="X23" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Y23" s="6"/>
       <c r="Z23" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AA23" s="6"/>
-      <c r="AB23" s="5" t="s">
-        <v>24</v>
+      <c r="AB23" s="19" t="s">
+        <v>38</v>
       </c>
       <c r="AC23" s="6"/>
       <c r="AD23" s="5" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="AE23" s="6"/>
-      <c r="AF23" s="15"/>
-      <c r="AG23" s="6"/>
-      <c r="AH23" s="15"/>
-      <c r="AI23" s="15"/>
-      <c r="AJ23" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="AK23" s="6"/>
-      <c r="AL23" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="AM23" s="7"/>
+      <c r="AF23" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG23" s="7"/>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D24" s="5">
         <v>27.19</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F24" s="5">
         <v>140.18</v>
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J24" s="5">
         <v>250</v>
@@ -3674,93 +3423,79 @@
       </c>
       <c r="O24" s="6"/>
       <c r="P24" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q24" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="Q24" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="R24" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S24" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="T24" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U24" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="V24" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="T24" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="U24" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="V24" s="15" t="s">
-        <v>93</v>
-      </c>
       <c r="W24" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="X24" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y24" s="6"/>
+        <v>53</v>
+      </c>
+      <c r="Y24" s="6" t="s">
+        <v>96</v>
+      </c>
       <c r="Z24" s="5" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="AA24" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="AB24" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC24" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AD24" s="5">
+        <v>103</v>
+      </c>
+      <c r="AB24" s="5">
         <v>20.75</v>
       </c>
+      <c r="AC24" s="6"/>
+      <c r="AD24" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="AE24" s="6"/>
-      <c r="AF24" s="15">
-        <v>0.13</v>
-      </c>
-      <c r="AG24" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH24" s="15">
-        <v>34.6</v>
-      </c>
-      <c r="AI24" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="AJ24" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK24" s="6"/>
-      <c r="AL24" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM24" s="7"/>
+      <c r="AF24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG24" s="7"/>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D25" s="5">
         <v>39.29</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F25" s="5">
         <v>45.47</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J25" s="5">
         <v>580</v>
@@ -3775,93 +3510,79 @@
       </c>
       <c r="O25" s="6"/>
       <c r="P25" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q25" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="Q25" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="R25" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="S25" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="T25" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="S25" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="T25" s="5" t="s">
+      <c r="U25" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="V25" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="W25" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="X25" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="U25" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="V25" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="W25" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="X25" s="5" t="s">
+      <c r="Y25" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="Y25" s="6"/>
-      <c r="Z25" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="AA25" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="AB25" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC25" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AD25" s="5">
+        <v>103</v>
+      </c>
+      <c r="AB25" s="5">
         <v>8.65</v>
       </c>
+      <c r="AC25" s="6"/>
+      <c r="AD25" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="AE25" s="6"/>
-      <c r="AF25" s="15">
-        <v>0.62</v>
-      </c>
-      <c r="AG25" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH25" s="15">
-        <v>25.5</v>
-      </c>
-      <c r="AI25" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="AJ25" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="AK25" s="6"/>
-      <c r="AL25" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="AM25" s="7"/>
+      <c r="AF25" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG25" s="7"/>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D26" s="5">
         <v>7.69</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F26" s="5">
         <v>37.950000000000003</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J26" s="5">
         <v>75</v>
@@ -3871,86 +3592,80 @@
         <v>57.6</v>
       </c>
       <c r="M26" s="6"/>
-      <c r="N26" s="5" t="s">
-        <v>41</v>
+      <c r="N26" s="19" t="s">
+        <v>38</v>
       </c>
       <c r="O26" s="6"/>
       <c r="P26" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q26" s="6"/>
+        <v>51</v>
+      </c>
+      <c r="Q26" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="R26" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S26" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="T26" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="U26" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="V26" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="T26" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="U26" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="V26" s="15" t="s">
-        <v>93</v>
-      </c>
       <c r="W26" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="X26" s="5" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="Y26" s="6"/>
       <c r="Z26" s="5" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="AA26" s="6"/>
-      <c r="AB26" s="5" t="s">
-        <v>24</v>
+      <c r="AB26" s="5">
+        <v>5</v>
       </c>
       <c r="AC26" s="6"/>
-      <c r="AD26" s="5">
-        <v>5</v>
+      <c r="AD26" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="AE26" s="6"/>
-      <c r="AF26" s="15"/>
-      <c r="AG26" s="6"/>
-      <c r="AH26" s="15"/>
-      <c r="AI26" s="15"/>
-      <c r="AJ26" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK26" s="6"/>
-      <c r="AL26" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM26" s="7"/>
+      <c r="AF26" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG26" s="7"/>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D27" s="5">
         <v>13.93</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F27" s="5">
         <v>104.95</v>
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J27" s="5">
         <v>70</v>
@@ -3965,91 +3680,77 @@
       </c>
       <c r="O27" s="6"/>
       <c r="P27" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q27" s="6"/>
+        <v>81</v>
+      </c>
+      <c r="Q27" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="R27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S27" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="T27" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="U27" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="V27" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="T27" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="U27" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="V27" s="15" t="s">
-        <v>93</v>
-      </c>
       <c r="W27" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="X27" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Y27" s="6"/>
       <c r="Z27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA27" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB27" s="5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AC27" s="6"/>
+      <c r="AD27" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="AA27" s="6"/>
-      <c r="AB27" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC27" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AD27" s="5">
-        <v>2.2000000000000002</v>
-      </c>
       <c r="AE27" s="6"/>
-      <c r="AF27" s="15">
-        <v>-0.77</v>
-      </c>
-      <c r="AG27" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH27" s="15">
-        <v>31.5</v>
-      </c>
-      <c r="AI27" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="AJ27" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK27" s="6"/>
-      <c r="AL27" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM27" s="7"/>
+      <c r="AF27" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG27" s="7"/>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D28" s="5">
         <v>41.89</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F28" s="5">
         <v>63.76</v>
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J28" s="5">
         <v>120</v>
@@ -4064,83 +3765,77 @@
       </c>
       <c r="O28" s="6"/>
       <c r="P28" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q28" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="Q28" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="R28" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="S28" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T28" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U28" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="V28" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="W28" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="X28" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y28" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z28" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="Y28" s="6"/>
-      <c r="Z28" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA28" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="AB28" s="5" t="s">
+      <c r="AA28" s="6"/>
+      <c r="AB28" s="5">
+        <v>2</v>
+      </c>
+      <c r="AC28" s="6"/>
+      <c r="AD28" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE28" s="6"/>
+      <c r="AF28" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AC28" s="6"/>
-      <c r="AD28" s="5">
-        <v>2</v>
-      </c>
-      <c r="AE28" s="6"/>
-      <c r="AF28" s="15"/>
-      <c r="AG28" s="6"/>
-      <c r="AH28" s="15"/>
-      <c r="AI28" s="15"/>
-      <c r="AJ28" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK28" s="6"/>
-      <c r="AL28" s="5" t="s">
+      <c r="AG28" s="7"/>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AM28" s="7"/>
-    </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A29" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="C29" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D29" s="5">
         <v>1.1299999999999999</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F29" s="5">
         <v>37.15</v>
       </c>
       <c r="G29" s="6"/>
       <c r="H29" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J29" s="5">
         <v>167</v>
@@ -4155,93 +3850,79 @@
       </c>
       <c r="O29" s="6"/>
       <c r="P29" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q29" s="6"/>
+        <v>51</v>
+      </c>
+      <c r="Q29" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="R29" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S29" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="T29" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="U29" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="V29" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="T29" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="U29" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="V29" s="15" t="s">
+      <c r="W29" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="X29" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y29" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="W29" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="X29" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y29" s="6"/>
       <c r="Z29" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA29" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB29" s="5">
+        <v>16.95</v>
+      </c>
+      <c r="AC29" s="6"/>
+      <c r="AD29" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE29" s="6"/>
+      <c r="AF29" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG29" s="7"/>
+    </row>
+    <row r="30" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AA29" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="AB29" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC29" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AD29" s="5">
-        <v>16.95</v>
-      </c>
-      <c r="AE29" s="6"/>
-      <c r="AF29" s="15">
-        <v>-0.25</v>
-      </c>
-      <c r="AG29" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH29" s="15">
-        <v>30.4</v>
-      </c>
-      <c r="AI29" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="AJ29" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK29" s="6"/>
-      <c r="AL29" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="AM29" s="7"/>
-    </row>
-    <row r="30" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="C30" s="10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D30" s="9">
         <v>17.66</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F30" s="9">
         <v>-49.17</v>
       </c>
       <c r="G30" s="10"/>
       <c r="H30" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J30" s="9">
         <v>134</v>
@@ -4256,67 +3937,53 @@
       </c>
       <c r="O30" s="10"/>
       <c r="P30" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q30" s="10"/>
+        <v>81</v>
+      </c>
+      <c r="Q30" s="10" t="s">
+        <v>107</v>
+      </c>
       <c r="R30" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S30" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="T30" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="U30" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="V30" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="T30" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="U30" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="V30" s="16" t="s">
-        <v>93</v>
-      </c>
       <c r="W30" s="10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="X30" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y30" s="10"/>
+        <v>34</v>
+      </c>
+      <c r="Y30" s="10" t="s">
+        <v>92</v>
+      </c>
       <c r="Z30" s="9" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="AA30" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="AB30" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC30" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="AD30" s="9">
+        <v>103</v>
+      </c>
+      <c r="AB30" s="9">
         <v>4.71</v>
       </c>
+      <c r="AC30" s="10"/>
+      <c r="AD30" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="AE30" s="10"/>
-      <c r="AF30" s="16">
-        <v>-0.19</v>
-      </c>
-      <c r="AG30" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH30" s="16">
-        <v>33.5</v>
-      </c>
-      <c r="AI30" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="AJ30" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK30" s="10"/>
-      <c r="AL30" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM30" s="11"/>
+      <c r="AF30" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG30" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>